<commit_message>
Presses added, with different form of monitoring and weird times
</commit_message>
<xml_diff>
--- a/workingTable/shifts_table.xlsx
+++ b/workingTable/shifts_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henrique.engelke\OneDrive - Martinrea Inc\Documents\GitHub\Scheduler\workingTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AFCF53-214D-406C-8B91-4B4BA9C7E040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9212B4-CC18-4867-BEC6-A3735584FE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="34">
   <si>
     <t>MARTINREA HFS</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Effective Length (Hrs)</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>ELCV</t>
   </si>
 </sst>
 </file>
@@ -1459,8 +1468,8 @@
   </sheetPr>
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G48"/>
+    <sheetView topLeftCell="A3" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1678,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="72"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
@@ -1723,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="72"/>
       <c r="B8" s="24" t="s">
         <v>17</v>
@@ -1768,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="72"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -1897,7 +1906,9 @@
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="58"/>
       <c r="E11" s="58"/>
       <c r="F11" s="58">
@@ -1935,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72"/>
       <c r="B12" s="19" t="s">
         <v>16</v>
@@ -1978,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="72"/>
       <c r="B13" s="24" t="s">
         <v>17</v>
@@ -2021,7 +2032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="72"/>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -2141,7 +2152,9 @@
       <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58">
@@ -2179,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="72"/>
       <c r="B17" s="19" t="s">
         <v>16</v>
@@ -2222,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="72"/>
       <c r="B18" s="24" t="s">
         <v>17</v>
@@ -2265,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="72"/>
       <c r="B19" s="29" t="s">
         <v>18</v>
@@ -2423,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="72"/>
       <c r="B22" s="19" t="s">
         <v>16</v>
@@ -2466,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="72"/>
       <c r="B23" s="24" t="s">
         <v>17</v>
@@ -2509,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="73"/>
       <c r="B24" s="29" t="s">
         <v>18</v>
@@ -2675,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="72"/>
       <c r="B27" s="19" t="s">
         <v>16</v>
@@ -2720,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="72"/>
       <c r="B28" s="24" t="s">
         <v>17</v>
@@ -2765,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="72"/>
       <c r="B29" s="29" t="s">
         <v>18</v>
@@ -2932,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="72"/>
       <c r="B32" s="19" t="s">
         <v>16</v>
@@ -2975,7 +2988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="72"/>
       <c r="B33" s="24" t="s">
         <v>17</v>
@@ -3018,7 +3031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="72"/>
       <c r="B34" s="29" t="s">
         <v>18</v>
@@ -3176,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="72"/>
       <c r="B37" s="19" t="s">
         <v>16</v>
@@ -3219,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="72"/>
       <c r="B38" s="24" t="s">
         <v>17</v>
@@ -3262,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="72"/>
       <c r="B39" s="29" t="s">
         <v>18</v>
@@ -3420,7 +3433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="72"/>
       <c r="B42" s="19" t="s">
         <v>16</v>
@@ -3463,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="72"/>
       <c r="B43" s="24" t="s">
         <v>17</v>
@@ -3506,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="73"/>
       <c r="B44" s="29" t="s">
         <v>18</v>
@@ -3672,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="72"/>
       <c r="B47" s="19" t="s">
         <v>16</v>
@@ -3717,7 +3730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="72"/>
       <c r="B48" s="24" t="s">
         <v>17</v>
@@ -3762,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="72"/>
       <c r="B49" s="29" t="s">
         <v>18</v>
@@ -3890,7 +3903,9 @@
       <c r="B51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="74" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="58">
@@ -3928,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="72"/>
       <c r="B52" s="19" t="s">
         <v>16</v>
@@ -3971,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="72"/>
       <c r="B53" s="24" t="s">
         <v>17</v>
@@ -4014,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="72"/>
       <c r="B54" s="29" t="s">
         <v>18</v>
@@ -4607,8 +4622,8 @@
   </sheetPr>
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G48"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4822,7 +4837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="72"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
@@ -4867,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="72"/>
       <c r="B8" s="24" t="s">
         <v>17</v>
@@ -4912,7 +4927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="72"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -5041,7 +5056,9 @@
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="58"/>
       <c r="E11" s="58"/>
       <c r="F11" s="58">
@@ -5079,7 +5096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72"/>
       <c r="B12" s="19" t="s">
         <v>16</v>
@@ -5122,7 +5139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="72"/>
       <c r="B13" s="24" t="s">
         <v>17</v>
@@ -5165,7 +5182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="72"/>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -5285,7 +5302,9 @@
       <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58">
@@ -5323,7 +5342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="72"/>
       <c r="B17" s="19" t="s">
         <v>16</v>
@@ -5366,7 +5385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="72"/>
       <c r="B18" s="24" t="s">
         <v>17</v>
@@ -5409,7 +5428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="72"/>
       <c r="B19" s="29" t="s">
         <v>18</v>
@@ -5567,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="72"/>
       <c r="B22" s="19" t="s">
         <v>16</v>
@@ -5610,7 +5629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="72"/>
       <c r="B23" s="24" t="s">
         <v>17</v>
@@ -5653,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="73"/>
       <c r="B24" s="29" t="s">
         <v>18</v>
@@ -5819,7 +5838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="72"/>
       <c r="B27" s="19" t="s">
         <v>16</v>
@@ -5864,7 +5883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="72"/>
       <c r="B28" s="24" t="s">
         <v>17</v>
@@ -5923,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="72"/>
       <c r="B29" s="29" t="s">
         <v>18</v>
@@ -6090,7 +6109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="72"/>
       <c r="B32" s="19" t="s">
         <v>16</v>
@@ -6133,7 +6152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="72"/>
       <c r="B33" s="24" t="s">
         <v>17</v>
@@ -6176,7 +6195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="72"/>
       <c r="B34" s="29" t="s">
         <v>18</v>
@@ -6334,7 +6353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="72"/>
       <c r="B37" s="19" t="s">
         <v>16</v>
@@ -6377,7 +6396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="72"/>
       <c r="B38" s="24" t="s">
         <v>17</v>
@@ -6420,7 +6439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="72"/>
       <c r="B39" s="29" t="s">
         <v>18</v>
@@ -6578,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="72"/>
       <c r="B42" s="19" t="s">
         <v>16</v>
@@ -6621,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="72"/>
       <c r="B43" s="24" t="s">
         <v>17</v>
@@ -6664,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="73"/>
       <c r="B44" s="29" t="s">
         <v>18</v>
@@ -6830,7 +6849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="72"/>
       <c r="B47" s="19" t="s">
         <v>16</v>
@@ -6875,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="72"/>
       <c r="B48" s="24" t="s">
         <v>17</v>
@@ -6920,7 +6939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="72"/>
       <c r="B49" s="29" t="s">
         <v>18</v>
@@ -7048,7 +7067,9 @@
       <c r="B51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="74" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="58">
@@ -7086,7 +7107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="72"/>
       <c r="B52" s="19" t="s">
         <v>16</v>
@@ -7129,7 +7150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="72"/>
       <c r="B53" s="24" t="s">
         <v>17</v>
@@ -7172,7 +7193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="72"/>
       <c r="B54" s="29" t="s">
         <v>18</v>
@@ -7765,8 +7786,8 @@
   </sheetPr>
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G48"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7980,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="72"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
@@ -8025,7 +8046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="72"/>
       <c r="B8" s="24" t="s">
         <v>17</v>
@@ -8070,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="72"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -8199,7 +8220,9 @@
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="58"/>
       <c r="E11" s="58"/>
       <c r="F11" s="58">
@@ -8237,7 +8260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72"/>
       <c r="B12" s="19" t="s">
         <v>16</v>
@@ -8280,7 +8303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="72"/>
       <c r="B13" s="24" t="s">
         <v>17</v>
@@ -8323,7 +8346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="72"/>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -8443,7 +8466,9 @@
       <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58">
@@ -8481,7 +8506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="72"/>
       <c r="B17" s="19" t="s">
         <v>16</v>
@@ -8524,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="72"/>
       <c r="B18" s="24" t="s">
         <v>17</v>
@@ -8567,7 +8592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="72"/>
       <c r="B19" s="29" t="s">
         <v>18</v>
@@ -8725,7 +8750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="72"/>
       <c r="B22" s="19" t="s">
         <v>16</v>
@@ -8768,7 +8793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="72"/>
       <c r="B23" s="24" t="s">
         <v>17</v>
@@ -8811,7 +8836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="73"/>
       <c r="B24" s="29" t="s">
         <v>18</v>
@@ -8977,7 +9002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="72"/>
       <c r="B27" s="19" t="s">
         <v>16</v>
@@ -9022,7 +9047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="72"/>
       <c r="B28" s="24" t="s">
         <v>17</v>
@@ -9067,7 +9092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="72"/>
       <c r="B29" s="29" t="s">
         <v>18</v>
@@ -9234,7 +9259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="72"/>
       <c r="B32" s="19" t="s">
         <v>16</v>
@@ -9277,7 +9302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="72"/>
       <c r="B33" s="24" t="s">
         <v>17</v>
@@ -9320,7 +9345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="72"/>
       <c r="B34" s="29" t="s">
         <v>18</v>
@@ -9478,7 +9503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="72"/>
       <c r="B37" s="19" t="s">
         <v>16</v>
@@ -9521,7 +9546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="72"/>
       <c r="B38" s="24" t="s">
         <v>17</v>
@@ -9564,7 +9589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="72"/>
       <c r="B39" s="29" t="s">
         <v>18</v>
@@ -9722,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="72"/>
       <c r="B42" s="19" t="s">
         <v>16</v>
@@ -9765,7 +9790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="72"/>
       <c r="B43" s="24" t="s">
         <v>17</v>
@@ -9808,7 +9833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="73"/>
       <c r="B44" s="29" t="s">
         <v>18</v>
@@ -9974,7 +9999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="72"/>
       <c r="B47" s="19" t="s">
         <v>16</v>
@@ -10019,7 +10044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="72"/>
       <c r="B48" s="24" t="s">
         <v>17</v>
@@ -10064,7 +10089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="72"/>
       <c r="B49" s="29" t="s">
         <v>18</v>
@@ -10192,7 +10217,9 @@
       <c r="B51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="74" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="58">
@@ -10230,7 +10257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="72"/>
       <c r="B52" s="19" t="s">
         <v>16</v>
@@ -10273,7 +10300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="72"/>
       <c r="B53" s="24" t="s">
         <v>17</v>
@@ -10316,7 +10343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="72"/>
       <c r="B54" s="29" t="s">
         <v>18</v>
@@ -10909,8 +10936,8 @@
   </sheetPr>
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11161,7 +11188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="72"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
@@ -11206,7 +11233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="72"/>
       <c r="B8" s="24" t="s">
         <v>17</v>
@@ -11251,7 +11278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="72"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -11380,7 +11407,9 @@
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="58"/>
       <c r="E11" s="58"/>
       <c r="F11" s="58">
@@ -11418,7 +11447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72"/>
       <c r="B12" s="19" t="s">
         <v>16</v>
@@ -11461,7 +11490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="72"/>
       <c r="B13" s="24" t="s">
         <v>17</v>
@@ -11504,7 +11533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="72"/>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -11624,7 +11653,9 @@
       <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58">
@@ -11662,7 +11693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="72"/>
       <c r="B17" s="19" t="s">
         <v>16</v>
@@ -11705,7 +11736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="72"/>
       <c r="B18" s="24" t="s">
         <v>17</v>
@@ -11748,7 +11779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="72"/>
       <c r="B19" s="29" t="s">
         <v>18</v>
@@ -11906,7 +11937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="72"/>
       <c r="B22" s="19" t="s">
         <v>16</v>
@@ -11949,7 +11980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="72"/>
       <c r="B23" s="24" t="s">
         <v>17</v>
@@ -11992,7 +12023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="73"/>
       <c r="B24" s="29" t="s">
         <v>18</v>
@@ -12158,7 +12189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="72"/>
       <c r="B27" s="19" t="s">
         <v>16</v>
@@ -12168,17 +12199,17 @@
         <v>7.5</v>
       </c>
       <c r="E27" s="49">
-        <v>4.7195555555555559</v>
+        <v>4.4235555555555557</v>
       </c>
       <c r="F27" s="58">
         <f t="shared" ref="F27:F28" si="18">D27-E27</f>
-        <v>2.7804444444444441</v>
+        <v>3.0764444444444443</v>
       </c>
       <c r="G27" s="15">
         <v>59.2</v>
       </c>
       <c r="H27" s="20">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="I27" s="16">
         <f>(D27*3600)/G27</f>
@@ -12186,83 +12217,97 @@
       </c>
       <c r="J27" s="16">
         <f>I27-H27</f>
-        <v>169.08108108108104</v>
+        <v>187.08108108108104</v>
       </c>
       <c r="K27" s="69">
         <f t="shared" ref="K27:K28" si="19">(N27+Q27)/D27</f>
-        <v>0.2870886790664115</v>
+        <v>0.32935457879172508</v>
       </c>
       <c r="L27" s="22">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="M27" s="53">
         <f>(N27/D27)*100%</f>
-        <v>0.17573587904506333</v>
+        <v>0.17242954753063419</v>
       </c>
       <c r="N27" s="48">
-        <v>1.3180190928379749</v>
+        <v>1.2932216064797564</v>
       </c>
       <c r="O27" s="23">
         <v>8</v>
       </c>
       <c r="P27" s="53">
         <f t="shared" ref="P27:P28" si="20">Q27/D27</f>
-        <v>0.11135280002134816</v>
+        <v>0.15692503126109086</v>
       </c>
       <c r="Q27" s="48">
-        <v>0.8351460001601112</v>
+        <v>1.1769377344581815</v>
       </c>
       <c r="R27" s="50">
         <f t="shared" ref="R27:R28" si="21">F27-(Q27+N27)</f>
-        <v>0.62727935144635794</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.60628510350650622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="72"/>
       <c r="B28" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="75"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="64"/>
+      <c r="D28" s="58">
+        <v>7.5</v>
+      </c>
+      <c r="E28" s="64">
+        <v>5.2786666666666671</v>
+      </c>
       <c r="F28" s="58">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2.2213333333333329</v>
       </c>
       <c r="G28" s="15">
         <v>59.2</v>
       </c>
-      <c r="H28" s="25"/>
+      <c r="H28" s="25">
+        <v>321</v>
+      </c>
       <c r="I28" s="16">
         <f>(D28*3600)/G28</f>
-        <v>0</v>
+        <v>456.08108108108104</v>
       </c>
       <c r="J28" s="16">
         <f>I28-H28</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="69" t="e">
+        <v>135.08108108108104</v>
+      </c>
+      <c r="K28" s="69">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L28" s="27"/>
-      <c r="M28" s="53" t="e">
+        <v>0.24886493937174581</v>
+      </c>
+      <c r="L28" s="27">
+        <v>282</v>
+      </c>
+      <c r="M28" s="53">
         <f>(N28/D28)*100%</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N28" s="62"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="53" t="e">
+        <v>0.20136456088136845</v>
+      </c>
+      <c r="N28" s="62">
+        <v>1.5102342066102634</v>
+      </c>
+      <c r="O28" s="28">
+        <v>3</v>
+      </c>
+      <c r="P28" s="53">
         <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q28" s="48"/>
+        <v>4.750037849037736E-2</v>
+      </c>
+      <c r="Q28" s="48">
+        <v>0.3562528386778302</v>
+      </c>
       <c r="R28" s="50">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.35484628804523943</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="72"/>
       <c r="B29" s="29" t="s">
         <v>18</v>
@@ -12270,28 +12315,28 @@
       <c r="C29" s="76"/>
       <c r="D29" s="65">
         <f>SUM(D26:D28)</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="E29" s="59">
         <f>SUM(E26:E28)</f>
-        <v>4.7195555555555559</v>
+        <v>9.7022222222222219</v>
       </c>
       <c r="F29" s="59">
         <f>SUM(F26:F28)</f>
-        <v>2.7804444444444441</v>
+        <v>5.2977777777777773</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="30">
         <f>SUM(H26:H28)</f>
-        <v>287</v>
+        <v>590</v>
       </c>
       <c r="I29" s="32">
         <f>SUM(I26:I28)</f>
-        <v>456.08108108108104</v>
+        <v>912.16216216216208</v>
       </c>
       <c r="J29" s="32">
         <f>SUM(J26:J28)</f>
-        <v>169.08108108108104</v>
+        <v>322.16216216216208</v>
       </c>
       <c r="K29" s="33" t="e">
         <f>AVERAGE(K26:K28)</f>
@@ -12299,16 +12344,16 @@
       </c>
       <c r="L29" s="34">
         <f>SUM(L26:L28)</f>
-        <v>192</v>
+        <v>487</v>
       </c>
       <c r="M29" s="52"/>
       <c r="N29" s="56">
         <f>SUM(N26:N28)</f>
-        <v>1.3180190928379749</v>
+        <v>2.8034558130900198</v>
       </c>
       <c r="O29" s="35">
         <f>SUM(O26:O28)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P29" s="54" t="e">
         <f>AVERAGE(P26:P28)</f>
@@ -12316,11 +12361,11 @@
       </c>
       <c r="Q29" s="56">
         <f>SUM(Q26:Q28)</f>
-        <v>0.8351460001601112</v>
+        <v>1.5331905731360118</v>
       </c>
       <c r="R29" s="56">
         <f>SUM(R26:R28)</f>
-        <v>0.62727935144635794</v>
+        <v>0.96113139155174565</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -12429,7 +12474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="72"/>
       <c r="B32" s="19" t="s">
         <v>16</v>
@@ -12472,7 +12517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="72"/>
       <c r="B33" s="24" t="s">
         <v>17</v>
@@ -12515,7 +12560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="72"/>
       <c r="B34" s="29" t="s">
         <v>18</v>
@@ -12673,7 +12718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="72"/>
       <c r="B37" s="19" t="s">
         <v>16</v>
@@ -12716,7 +12761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="72"/>
       <c r="B38" s="24" t="s">
         <v>17</v>
@@ -12759,7 +12804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="72"/>
       <c r="B39" s="29" t="s">
         <v>18</v>
@@ -12917,7 +12962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="72"/>
       <c r="B42" s="19" t="s">
         <v>16</v>
@@ -12960,7 +13005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="72"/>
       <c r="B43" s="24" t="s">
         <v>17</v>
@@ -13003,7 +13048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="73"/>
       <c r="B44" s="29" t="s">
         <v>18</v>
@@ -13169,97 +13214,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="72"/>
       <c r="B47" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C47" s="75"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="49"/>
+      <c r="D47" s="58">
+        <v>6.296170289648904</v>
+      </c>
+      <c r="E47" s="49">
+        <v>4.4400000000000004</v>
+      </c>
       <c r="F47" s="58">
         <f t="shared" ref="F47:F48" si="36">D47-E47</f>
-        <v>0</v>
+        <v>1.8561702896489036</v>
       </c>
       <c r="G47" s="21">
         <v>48</v>
       </c>
-      <c r="H47" s="20"/>
+      <c r="H47" s="20">
+        <v>333</v>
+      </c>
       <c r="I47" s="16">
         <f>(D47*3600)/G47</f>
-        <v>0</v>
+        <v>472.2127717236678</v>
       </c>
       <c r="J47" s="16">
         <f>I47-H47</f>
-        <v>0</v>
-      </c>
-      <c r="K47" s="69" t="e">
+        <v>139.2127717236678</v>
+      </c>
+      <c r="K47" s="69">
         <f t="shared" ref="K47:K48" si="37">(N47+Q47)/D47</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L47" s="22"/>
-      <c r="M47" s="53" t="e">
+        <v>0.32457912592130073</v>
+      </c>
+      <c r="L47" s="22">
+        <v>141</v>
+      </c>
+      <c r="M47" s="53">
         <f>(N47/D47)*100%</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N47" s="48"/>
-      <c r="O47" s="23"/>
-      <c r="P47" s="53" t="e">
+        <v>0.19103395860560735</v>
+      </c>
+      <c r="N47" s="48">
+        <v>1.2027823344866435</v>
+      </c>
+      <c r="O47" s="23">
+        <v>5</v>
+      </c>
+      <c r="P47" s="53">
         <f t="shared" ref="P47:P48" si="38">Q47/D47</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q47" s="48"/>
+        <v>0.13354516731569335</v>
+      </c>
+      <c r="Q47" s="48">
+        <v>0.84082311477926042</v>
+      </c>
       <c r="R47" s="50">
         <f t="shared" ref="R47:R48" si="39">F47-(Q47+N47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-0.1874351596170003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="72"/>
       <c r="B48" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C48" s="75"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="64"/>
+      <c r="D48" s="58">
+        <v>7.5</v>
+      </c>
+      <c r="E48" s="64">
+        <v>5.04</v>
+      </c>
       <c r="F48" s="58">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>2.46</v>
       </c>
       <c r="G48" s="26">
         <v>48</v>
       </c>
-      <c r="H48" s="25"/>
+      <c r="H48" s="25">
+        <v>378</v>
+      </c>
       <c r="I48" s="16">
         <f>(D48*3600)/G48</f>
-        <v>0</v>
+        <v>562.5</v>
       </c>
       <c r="J48" s="16">
         <f>I48-H48</f>
-        <v>0</v>
-      </c>
-      <c r="K48" s="69" t="e">
+        <v>184.5</v>
+      </c>
+      <c r="K48" s="69">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L48" s="27"/>
-      <c r="M48" s="53" t="e">
+        <v>4.8887504259745279E-2</v>
+      </c>
+      <c r="L48" s="27">
+        <v>22</v>
+      </c>
+      <c r="M48" s="53">
         <f>(N48/D48)*100%</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N48" s="62"/>
-      <c r="O48" s="28"/>
-      <c r="P48" s="53" t="e">
+        <v>3.8190607706705723E-2</v>
+      </c>
+      <c r="N48" s="62">
+        <v>0.28642955780029294</v>
+      </c>
+      <c r="O48" s="28">
+        <v>1</v>
+      </c>
+      <c r="P48" s="53">
         <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q48" s="48"/>
+        <v>1.0696896553039551E-2</v>
+      </c>
+      <c r="Q48" s="48">
+        <v>8.0226724147796635E-2</v>
+      </c>
       <c r="R48" s="50">
         <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2.0933437180519103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="72"/>
       <c r="B49" s="29" t="s">
         <v>18</v>
@@ -13267,28 +13340,28 @@
       <c r="C49" s="76"/>
       <c r="D49" s="65">
         <f>SUM(D46:D48)</f>
-        <v>0</v>
+        <v>13.796170289648904</v>
       </c>
       <c r="E49" s="59">
         <f>SUM(E46:E48)</f>
-        <v>0</v>
+        <v>9.48</v>
       </c>
       <c r="F49" s="59">
         <f>SUM(F46:F48)</f>
-        <v>0</v>
+        <v>4.3161702896489036</v>
       </c>
       <c r="G49" s="31"/>
       <c r="H49" s="30">
         <f>SUM(H46:H48)</f>
-        <v>0</v>
+        <v>711</v>
       </c>
       <c r="I49" s="32">
         <f>SUM(I46:I48)</f>
-        <v>0</v>
+        <v>1034.7127717236679</v>
       </c>
       <c r="J49" s="32">
         <f>SUM(J46:J48)</f>
-        <v>0</v>
+        <v>323.7127717236678</v>
       </c>
       <c r="K49" s="33" t="e">
         <f>AVERAGE(K46:K48)</f>
@@ -13296,16 +13369,16 @@
       </c>
       <c r="L49" s="34">
         <f>SUM(L46:L48)</f>
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="M49" s="52"/>
       <c r="N49" s="56">
         <f>SUM(N46:N48)</f>
-        <v>0</v>
+        <v>1.4892118922869364</v>
       </c>
       <c r="O49" s="35">
         <f>SUM(O46:O48)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P49" s="54" t="e">
         <f>AVERAGE(P46:P48)</f>
@@ -13313,11 +13386,11 @@
       </c>
       <c r="Q49" s="56">
         <f>SUM(Q46:Q48)</f>
-        <v>0</v>
+        <v>0.92104983892705705</v>
       </c>
       <c r="R49" s="56">
         <f>SUM(R46:R48)</f>
-        <v>0</v>
+        <v>1.90590855843491</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -13387,7 +13460,9 @@
       <c r="B51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="74" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="58">
@@ -13425,7 +13500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="72"/>
       <c r="B52" s="19" t="s">
         <v>16</v>
@@ -13468,7 +13543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="72"/>
       <c r="B53" s="24" t="s">
         <v>17</v>
@@ -13511,7 +13586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="72"/>
       <c r="B54" s="29" t="s">
         <v>18</v>
@@ -14105,8 +14180,8 @@
   </sheetPr>
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14320,7 +14395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="72"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
@@ -14365,7 +14440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="72"/>
       <c r="B8" s="24" t="s">
         <v>17</v>
@@ -14410,7 +14485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="72"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -14539,7 +14614,9 @@
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="58"/>
       <c r="E11" s="58"/>
       <c r="F11" s="58">
@@ -14577,7 +14654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72"/>
       <c r="B12" s="19" t="s">
         <v>16</v>
@@ -14620,7 +14697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="72"/>
       <c r="B13" s="24" t="s">
         <v>17</v>
@@ -14663,7 +14740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="72"/>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -14783,7 +14860,9 @@
       <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58">
@@ -14821,7 +14900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="72"/>
       <c r="B17" s="19" t="s">
         <v>16</v>
@@ -14864,7 +14943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="72"/>
       <c r="B18" s="24" t="s">
         <v>17</v>
@@ -14907,7 +14986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="72"/>
       <c r="B19" s="29" t="s">
         <v>18</v>
@@ -15065,7 +15144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="72"/>
       <c r="B22" s="19" t="s">
         <v>16</v>
@@ -15108,7 +15187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="72"/>
       <c r="B23" s="24" t="s">
         <v>17</v>
@@ -15151,7 +15230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="73"/>
       <c r="B24" s="29" t="s">
         <v>18</v>
@@ -15317,66 +15396,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="72"/>
       <c r="B27" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="75"/>
-      <c r="D27" s="58">
-        <v>7.5</v>
-      </c>
-      <c r="E27" s="49">
-        <v>4.8511111111111109</v>
-      </c>
+      <c r="D27" s="58"/>
+      <c r="E27" s="49"/>
       <c r="F27" s="58">
         <f t="shared" ref="F27:F28" si="18">D27-E27</f>
-        <v>2.6488888888888891</v>
+        <v>0</v>
       </c>
       <c r="G27" s="15">
         <v>59.2</v>
       </c>
-      <c r="H27" s="20">
-        <v>295</v>
-      </c>
+      <c r="H27" s="20"/>
       <c r="I27" s="16">
         <f>(D27*3600)/G27</f>
-        <v>456.08108108108104</v>
+        <v>0</v>
       </c>
       <c r="J27" s="16">
         <f>I27-H27</f>
-        <v>161.08108108108104</v>
-      </c>
-      <c r="K27" s="69">
+        <v>0</v>
+      </c>
+      <c r="K27" s="69" t="e">
         <f t="shared" ref="K27:K28" si="19">(N27+Q27)/D27</f>
-        <v>0.27632635568689506</v>
-      </c>
-      <c r="L27" s="22">
-        <v>238</v>
-      </c>
-      <c r="M27" s="53">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L27" s="22"/>
+      <c r="M27" s="53" t="e">
         <f>(N27/D27)*100%</f>
-        <v>0.20260360261775917</v>
-      </c>
-      <c r="N27" s="48">
-        <v>1.5195270196331938</v>
-      </c>
-      <c r="O27" s="23">
-        <v>7</v>
-      </c>
-      <c r="P27" s="53">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N27" s="48"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="53" t="e">
         <f t="shared" ref="P27:P28" si="20">Q27/D27</f>
-        <v>7.3722753069135866E-2</v>
-      </c>
-      <c r="Q27" s="48">
-        <v>0.55292064801851903</v>
-      </c>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q27" s="48"/>
       <c r="R27" s="50">
         <f t="shared" ref="R27:R28" si="21">F27-(Q27+N27)</f>
-        <v>0.57644122123717612</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="72"/>
       <c r="B28" s="24" t="s">
         <v>17</v>
@@ -15421,7 +15486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="72"/>
       <c r="B29" s="29" t="s">
         <v>18</v>
@@ -15429,28 +15494,28 @@
       <c r="C29" s="76"/>
       <c r="D29" s="65">
         <f>SUM(D26:D28)</f>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="E29" s="59">
         <f>SUM(E26:E28)</f>
-        <v>4.8511111111111109</v>
+        <v>0</v>
       </c>
       <c r="F29" s="59">
         <f>SUM(F26:F28)</f>
-        <v>2.6488888888888891</v>
+        <v>0</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="30">
         <f>SUM(H26:H28)</f>
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="I29" s="32">
         <f>SUM(I26:I28)</f>
-        <v>456.08108108108104</v>
+        <v>0</v>
       </c>
       <c r="J29" s="32">
         <f>SUM(J26:J28)</f>
-        <v>161.08108108108104</v>
+        <v>0</v>
       </c>
       <c r="K29" s="33" t="e">
         <f>AVERAGE(K26:K28)</f>
@@ -15458,16 +15523,16 @@
       </c>
       <c r="L29" s="34">
         <f>SUM(L26:L28)</f>
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="M29" s="52"/>
       <c r="N29" s="56">
         <f>SUM(N26:N28)</f>
-        <v>1.5195270196331938</v>
+        <v>0</v>
       </c>
       <c r="O29" s="35">
         <f>SUM(O26:O28)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P29" s="54" t="e">
         <f>AVERAGE(P26:P28)</f>
@@ -15475,11 +15540,11 @@
       </c>
       <c r="Q29" s="56">
         <f>SUM(Q26:Q28)</f>
-        <v>0.55292064801851903</v>
+        <v>0</v>
       </c>
       <c r="R29" s="56">
         <f>SUM(R26:R28)</f>
-        <v>0.57644122123717612</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15588,7 +15653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="72"/>
       <c r="B32" s="19" t="s">
         <v>16</v>
@@ -15631,7 +15696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="72"/>
       <c r="B33" s="24" t="s">
         <v>17</v>
@@ -15674,7 +15739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="72"/>
       <c r="B34" s="29" t="s">
         <v>18</v>
@@ -15832,7 +15897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="72"/>
       <c r="B37" s="19" t="s">
         <v>16</v>
@@ -15875,7 +15940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="72"/>
       <c r="B38" s="24" t="s">
         <v>17</v>
@@ -15918,7 +15983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="72"/>
       <c r="B39" s="29" t="s">
         <v>18</v>
@@ -16076,7 +16141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="72"/>
       <c r="B42" s="19" t="s">
         <v>16</v>
@@ -16119,7 +16184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="72"/>
       <c r="B43" s="24" t="s">
         <v>17</v>
@@ -16162,7 +16227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="73"/>
       <c r="B44" s="29" t="s">
         <v>18</v>
@@ -16328,7 +16393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="72"/>
       <c r="B47" s="19" t="s">
         <v>16</v>
@@ -16373,7 +16438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="72"/>
       <c r="B48" s="24" t="s">
         <v>17</v>
@@ -16418,7 +16483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="72"/>
       <c r="B49" s="29" t="s">
         <v>18</v>
@@ -16546,7 +16611,9 @@
       <c r="B51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="74" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="58">
@@ -16584,7 +16651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="72"/>
       <c r="B52" s="19" t="s">
         <v>16</v>
@@ -16627,7 +16694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="72"/>
       <c r="B53" s="24" t="s">
         <v>17</v>
@@ -16670,7 +16737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="72"/>
       <c r="B54" s="29" t="s">
         <v>18</v>
@@ -17263,8 +17330,8 @@
   </sheetPr>
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G48"/>
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="C51" sqref="C6:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17697,7 +17764,9 @@
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="58"/>
       <c r="E11" s="58"/>
       <c r="F11" s="58">
@@ -17941,7 +18010,9 @@
       <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58">
@@ -19732,7 +19803,9 @@
       <c r="B51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="74" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="58">
@@ -20446,8 +20519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025C4095-B736-4F0D-A83E-FB76969E7CED}">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20645,7 +20718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="72"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
@@ -20690,7 +20763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="72"/>
       <c r="B8" s="24" t="s">
         <v>17</v>
@@ -20735,7 +20808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="72"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -20864,7 +20937,9 @@
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="58"/>
       <c r="E11" s="58"/>
       <c r="F11" s="58">
@@ -20902,7 +20977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72"/>
       <c r="B12" s="19" t="s">
         <v>16</v>
@@ -20945,7 +21020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="72"/>
       <c r="B13" s="24" t="s">
         <v>17</v>
@@ -20988,7 +21063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="72"/>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -21108,7 +21183,9 @@
       <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58">
@@ -21146,7 +21223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="72"/>
       <c r="B17" s="19" t="s">
         <v>16</v>
@@ -21189,7 +21266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="72"/>
       <c r="B18" s="24" t="s">
         <v>17</v>
@@ -21232,7 +21309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="72"/>
       <c r="B19" s="29" t="s">
         <v>18</v>
@@ -21390,7 +21467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="72"/>
       <c r="B22" s="19" t="s">
         <v>16</v>
@@ -21433,7 +21510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="72"/>
       <c r="B23" s="24" t="s">
         <v>17</v>
@@ -21476,7 +21553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="73"/>
       <c r="B24" s="29" t="s">
         <v>18</v>
@@ -21656,7 +21733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="72"/>
       <c r="B27" s="19" t="s">
         <v>16</v>
@@ -21715,7 +21792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="72"/>
       <c r="B28" s="24" t="s">
         <v>17</v>
@@ -21774,7 +21851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="72"/>
       <c r="B29" s="29" t="s">
         <v>18</v>
@@ -21941,7 +22018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="72"/>
       <c r="B32" s="19" t="s">
         <v>16</v>
@@ -21984,7 +22061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="72"/>
       <c r="B33" s="24" t="s">
         <v>17</v>
@@ -22027,7 +22104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="72"/>
       <c r="B34" s="29" t="s">
         <v>18</v>
@@ -22185,7 +22262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="72"/>
       <c r="B37" s="19" t="s">
         <v>16</v>
@@ -22228,7 +22305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="72"/>
       <c r="B38" s="24" t="s">
         <v>17</v>
@@ -22271,7 +22348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="72"/>
       <c r="B39" s="29" t="s">
         <v>18</v>
@@ -22429,7 +22506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="72"/>
       <c r="B42" s="19" t="s">
         <v>16</v>
@@ -22472,7 +22549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="72"/>
       <c r="B43" s="24" t="s">
         <v>17</v>
@@ -22515,7 +22592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="73"/>
       <c r="B44" s="29" t="s">
         <v>18</v>
@@ -22681,7 +22758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="72"/>
       <c r="B47" s="19" t="s">
         <v>16</v>
@@ -22726,7 +22803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="72"/>
       <c r="B48" s="24" t="s">
         <v>17</v>
@@ -22771,7 +22848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="72"/>
       <c r="B49" s="29" t="s">
         <v>18</v>
@@ -22899,7 +22976,9 @@
       <c r="B51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="74" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="58">
@@ -22937,7 +23016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="72"/>
       <c r="B52" s="19" t="s">
         <v>16</v>
@@ -22980,7 +23059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="72"/>
       <c r="B53" s="24" t="s">
         <v>17</v>
@@ -23023,7 +23102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="72"/>
       <c r="B54" s="29" t="s">
         <v>18</v>
@@ -23613,8 +23692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A183CAA-4958-4441-AB23-468713AB7CE4}">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G48"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23812,7 +23891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="72"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
@@ -23857,7 +23936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="72"/>
       <c r="B8" s="24" t="s">
         <v>17</v>
@@ -23902,7 +23981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="72"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -24031,7 +24110,9 @@
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="58"/>
       <c r="E11" s="58"/>
       <c r="F11" s="58">
@@ -24069,7 +24150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="72"/>
       <c r="B12" s="19" t="s">
         <v>16</v>
@@ -24112,7 +24193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="72"/>
       <c r="B13" s="24" t="s">
         <v>17</v>
@@ -24155,7 +24236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="72"/>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -24275,7 +24356,9 @@
       <c r="B16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="74"/>
+      <c r="C16" s="74" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58">
@@ -24313,7 +24396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="72"/>
       <c r="B17" s="19" t="s">
         <v>16</v>
@@ -24356,7 +24439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="72"/>
       <c r="B18" s="24" t="s">
         <v>17</v>
@@ -24399,7 +24482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="72"/>
       <c r="B19" s="29" t="s">
         <v>18</v>
@@ -24557,7 +24640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="72"/>
       <c r="B22" s="19" t="s">
         <v>16</v>
@@ -24600,7 +24683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="72"/>
       <c r="B23" s="24" t="s">
         <v>17</v>
@@ -24643,7 +24726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="73"/>
       <c r="B24" s="29" t="s">
         <v>18</v>
@@ -24823,7 +24906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="72"/>
       <c r="B27" s="19" t="s">
         <v>16</v>
@@ -24882,7 +24965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="72"/>
       <c r="B28" s="24" t="s">
         <v>17</v>
@@ -24941,7 +25024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="72"/>
       <c r="B29" s="29" t="s">
         <v>18</v>
@@ -25108,7 +25191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="72"/>
       <c r="B32" s="19" t="s">
         <v>16</v>
@@ -25151,7 +25234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="72"/>
       <c r="B33" s="24" t="s">
         <v>17</v>
@@ -25194,7 +25277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="72"/>
       <c r="B34" s="29" t="s">
         <v>18</v>
@@ -25352,7 +25435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="72"/>
       <c r="B37" s="19" t="s">
         <v>16</v>
@@ -25395,7 +25478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="72"/>
       <c r="B38" s="24" t="s">
         <v>17</v>
@@ -25438,7 +25521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="72"/>
       <c r="B39" s="29" t="s">
         <v>18</v>
@@ -25596,7 +25679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="72"/>
       <c r="B42" s="19" t="s">
         <v>16</v>
@@ -25639,7 +25722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="72"/>
       <c r="B43" s="24" t="s">
         <v>17</v>
@@ -25682,7 +25765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="73"/>
       <c r="B44" s="29" t="s">
         <v>18</v>
@@ -25848,7 +25931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="72"/>
       <c r="B47" s="19" t="s">
         <v>16</v>
@@ -25893,7 +25976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="72"/>
       <c r="B48" s="24" t="s">
         <v>17</v>
@@ -25938,7 +26021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="72"/>
       <c r="B49" s="29" t="s">
         <v>18</v>
@@ -26066,7 +26149,9 @@
       <c r="B51" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="74" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" s="58"/>
       <c r="E51" s="58"/>
       <c r="F51" s="58">
@@ -26104,7 +26189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="72"/>
       <c r="B52" s="19" t="s">
         <v>16</v>
@@ -26147,7 +26232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A53" s="72"/>
       <c r="B53" s="24" t="s">
         <v>17</v>
@@ -26190,7 +26275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="72"/>
       <c r="B54" s="29" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Count responds better when it is None
</commit_message>
<xml_diff>
--- a/workingTable/shifts_table.xlsx
+++ b/workingTable/shifts_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henrique.engelke\OneDrive - Martinrea Inc\Documents\GitHub\Scheduler\workingTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{937AC12D-AF28-40EA-85CF-C2E0AD30E4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C77F6DCA-AF21-4603-8AE1-F2244BA18EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17268" windowHeight="10608" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17268" windowHeight="10608" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week" sheetId="1" r:id="rId1"/>
@@ -7706,7 +7706,9 @@
         <v>17</v>
       </c>
       <c r="C8" s="103"/>
-      <c r="D8" s="58"/>
+      <c r="D8" s="58">
+        <v>6.0441144407457772</v>
+      </c>
       <c r="E8" s="64"/>
       <c r="F8" s="58"/>
       <c r="G8" s="26"/>
@@ -7730,7 +7732,7 @@
       <c r="C9" s="104"/>
       <c r="D9" s="65">
         <f>SUM(D6:D8)</f>
-        <v>12</v>
+        <v>18.044114440745776</v>
       </c>
       <c r="E9" s="59">
         <f>SUM(E6:E8)</f>
@@ -7892,7 +7894,9 @@
         <v>17</v>
       </c>
       <c r="C13" s="103"/>
-      <c r="D13" s="58"/>
+      <c r="D13" s="58">
+        <v>0</v>
+      </c>
       <c r="E13" s="64"/>
       <c r="F13" s="58"/>
       <c r="G13" s="26"/>
@@ -8025,7 +8029,9 @@
       <c r="C16" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="58"/>
+      <c r="D16" s="58">
+        <v>6.1211657509538862</v>
+      </c>
       <c r="E16" s="58"/>
       <c r="F16" s="58"/>
       <c r="G16" s="15"/>
@@ -8069,7 +8075,9 @@
         <v>17</v>
       </c>
       <c r="C18" s="103"/>
-      <c r="D18" s="58"/>
+      <c r="D18" s="58">
+        <v>7.5</v>
+      </c>
       <c r="E18" s="64"/>
       <c r="F18" s="58"/>
       <c r="G18" s="26"/>
@@ -8093,7 +8101,7 @@
       <c r="C19" s="104"/>
       <c r="D19" s="65">
         <f>SUM(D16:D18)</f>
-        <v>0</v>
+        <v>13.621165750953885</v>
       </c>
       <c r="E19" s="59">
         <f>SUM(E16:E18)</f>
@@ -8451,56 +8459,56 @@
         <v>21</v>
       </c>
       <c r="D26" s="58">
-        <v>12</v>
+        <v>7.5</v>
       </c>
       <c r="E26" s="58">
-        <v>10</v>
+        <v>1.6444444444444446E-2</v>
       </c>
       <c r="F26" s="58">
         <f>D26-E26</f>
-        <v>2</v>
+        <v>7.4835555555555553</v>
       </c>
       <c r="G26" s="15">
         <v>59.2</v>
       </c>
       <c r="H26" s="14">
-        <v>255</v>
+        <v>1</v>
       </c>
       <c r="I26" s="16">
         <f>(D26*3600)/G26</f>
-        <v>729.72972972972968</v>
+        <v>456.08108108108104</v>
       </c>
       <c r="J26" s="16">
         <f>I26-H26</f>
-        <v>474.72972972972968</v>
+        <v>455.08108108108104</v>
       </c>
       <c r="K26" s="69">
         <f>(N26+Q26)/D26</f>
-        <v>2.4189814814814817E-2</v>
+        <v>0</v>
       </c>
       <c r="L26" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="53">
         <f>(N26/D26)*100%</f>
-        <v>8.2638888888888883E-3</v>
+        <v>0</v>
       </c>
       <c r="N26" s="50">
-        <v>9.9166666666666667E-2</v>
+        <v>0</v>
       </c>
       <c r="O26" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P26" s="53">
         <f>Q26/D26</f>
-        <v>1.5925925925925927E-2</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="50">
-        <v>0.19111111111111112</v>
+        <v>0</v>
       </c>
       <c r="R26" s="50">
         <f>F26-(Q26+N26)</f>
-        <v>1.7097222222222221</v>
+        <v>7.4835555555555553</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8510,56 +8518,56 @@
       </c>
       <c r="C27" s="103"/>
       <c r="D27" s="58">
-        <v>12</v>
+        <v>7.5</v>
       </c>
       <c r="E27" s="49">
-        <v>10</v>
+        <v>5.1964444444444444</v>
       </c>
       <c r="F27" s="58">
         <f t="shared" ref="F27:F28" si="6">D27-E27</f>
-        <v>2</v>
+        <v>2.3035555555555556</v>
       </c>
       <c r="G27" s="15">
         <v>59.2</v>
       </c>
       <c r="H27" s="20">
-        <v>255</v>
+        <v>316</v>
       </c>
       <c r="I27" s="16">
         <f>(D27*3600)/G27</f>
-        <v>729.72972972972968</v>
+        <v>456.08108108108104</v>
       </c>
       <c r="J27" s="16">
         <f>I27-H27</f>
-        <v>474.72972972972968</v>
+        <v>140.08108108108104</v>
       </c>
       <c r="K27" s="69">
         <f t="shared" ref="K27:K28" si="7">(N27+Q27)/D27</f>
-        <v>2.4189814814814817E-2</v>
+        <v>0.25354902999136281</v>
       </c>
       <c r="L27" s="22">
-        <v>1</v>
+        <v>249</v>
       </c>
       <c r="M27" s="53">
         <f>(N27/D27)*100%</f>
-        <v>8.2638888888888883E-3</v>
+        <v>0.20748065957140135</v>
       </c>
       <c r="N27" s="48">
-        <v>9.9166666666666667E-2</v>
+        <v>1.5561049467855101</v>
       </c>
       <c r="O27" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P27" s="53">
         <f t="shared" ref="P27:P28" si="8">Q27/D27</f>
-        <v>1.5925925925925927E-2</v>
+        <v>4.6068370419961438E-2</v>
       </c>
       <c r="Q27" s="48">
-        <v>0.19111111111111112</v>
+        <v>0.34551277814971076</v>
       </c>
       <c r="R27" s="50">
         <f t="shared" ref="R27:R28" si="9">F27-(Q27+N27)</f>
-        <v>1.7097222222222221</v>
+        <v>0.40193783062033472</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8568,43 +8576,57 @@
         <v>17</v>
       </c>
       <c r="C28" s="103"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="64"/>
+      <c r="D28" s="58">
+        <v>7.5</v>
+      </c>
+      <c r="E28" s="64">
+        <v>4.4235555555555557</v>
+      </c>
       <c r="F28" s="58">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.0764444444444443</v>
       </c>
       <c r="G28" s="15">
         <v>59.2</v>
       </c>
-      <c r="H28" s="25"/>
+      <c r="H28" s="25">
+        <v>269</v>
+      </c>
       <c r="I28" s="16">
         <f>(D28*3600)/G28</f>
-        <v>0</v>
+        <v>456.08108108108104</v>
       </c>
       <c r="J28" s="16">
         <f>I28-H28</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="69" t="e">
+        <v>187.08108108108104</v>
+      </c>
+      <c r="K28" s="69">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L28" s="27"/>
-      <c r="M28" s="53" t="e">
+        <v>0.36362979921764887</v>
+      </c>
+      <c r="L28" s="27">
+        <v>237</v>
+      </c>
+      <c r="M28" s="53">
         <f>(N28/D28)*100%</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N28" s="62"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="53" t="e">
+        <v>0.24856649652587129</v>
+      </c>
+      <c r="N28" s="62">
+        <v>1.8642487239440346</v>
+      </c>
+      <c r="O28" s="28">
+        <v>9</v>
+      </c>
+      <c r="P28" s="53">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q28" s="48"/>
+        <v>0.11506330269177757</v>
+      </c>
+      <c r="Q28" s="48">
+        <v>0.8629747701883318</v>
+      </c>
       <c r="R28" s="50">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.34922095031207778</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8615,57 +8637,57 @@
       <c r="C29" s="104"/>
       <c r="D29" s="65">
         <f>SUM(D26:D28)</f>
-        <v>24</v>
+        <v>22.5</v>
       </c>
       <c r="E29" s="59">
         <f>SUM(E26:E28)</f>
-        <v>20</v>
+        <v>9.6364444444444448</v>
       </c>
       <c r="F29" s="59">
         <f>SUM(F26:F28)</f>
-        <v>4</v>
+        <v>12.863555555555555</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="30">
         <f>SUM(H26:H28)</f>
-        <v>510</v>
+        <v>586</v>
       </c>
       <c r="I29" s="32">
         <f>SUM(I26:I28)</f>
-        <v>1459.4594594594594</v>
+        <v>1368.2432432432431</v>
       </c>
       <c r="J29" s="32">
         <f>SUM(J26:J28)</f>
-        <v>949.45945945945937</v>
-      </c>
-      <c r="K29" s="33" t="e">
+        <v>782.24324324324311</v>
+      </c>
+      <c r="K29" s="33">
         <f>AVERAGE(K26:K28)</f>
-        <v>#DIV/0!</v>
+        <v>0.20572627640300389</v>
       </c>
       <c r="L29" s="34">
         <f>SUM(L26:L28)</f>
-        <v>2</v>
+        <v>486</v>
       </c>
       <c r="M29" s="52"/>
       <c r="N29" s="56">
         <f>SUM(N26:N28)</f>
-        <v>0.19833333333333333</v>
+        <v>3.4203536707295448</v>
       </c>
       <c r="O29" s="35">
         <f>SUM(O26:O28)</f>
-        <v>4</v>
-      </c>
-      <c r="P29" s="54" t="e">
+        <v>13</v>
+      </c>
+      <c r="P29" s="54">
         <f>AVERAGE(P26:P28)</f>
-        <v>#DIV/0!</v>
+        <v>5.3710557703913003E-2</v>
       </c>
       <c r="Q29" s="56">
         <f>SUM(Q26:Q28)</f>
-        <v>0.38222222222222224</v>
+        <v>1.2084875483380426</v>
       </c>
       <c r="R29" s="56">
         <f>SUM(R26:R28)</f>
-        <v>3.4194444444444443</v>
+        <v>8.2347143364879685</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9735,43 +9757,57 @@
       <c r="C51" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
+      <c r="D51" s="58">
+        <v>0</v>
+      </c>
+      <c r="E51" s="58">
+        <v>7.9118333333333331</v>
+      </c>
       <c r="F51" s="58">
         <f>D51-E51</f>
-        <v>0</v>
+        <v>-7.9118333333333331</v>
       </c>
       <c r="G51" s="15">
         <v>384.9</v>
       </c>
-      <c r="H51" s="14"/>
+      <c r="H51" s="14">
+        <v>74</v>
+      </c>
       <c r="I51" s="16">
         <f>(D51*3600)/G51</f>
         <v>0</v>
       </c>
       <c r="J51" s="16">
         <f>I51-H51</f>
-        <v>0</v>
+        <v>-74</v>
       </c>
       <c r="K51" s="69" t="e">
         <f>(N51+Q51)/D51</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L51" s="17"/>
+      <c r="L51" s="17">
+        <v>0</v>
+      </c>
       <c r="M51" s="53" t="e">
         <f>(N51/D51)*100%</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N51" s="50"/>
-      <c r="O51" s="18"/>
+      <c r="N51" s="50">
+        <v>0</v>
+      </c>
+      <c r="O51" s="18">
+        <v>0</v>
+      </c>
       <c r="P51" s="53" t="e">
         <f>Q51/D51</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q51" s="50"/>
+      <c r="Q51" s="50">
+        <v>0</v>
+      </c>
       <c r="R51" s="50">
         <f>F51-(Q51+N51)</f>
-        <v>0</v>
+        <v>-7.9118333333333331</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9780,43 +9816,57 @@
         <v>16</v>
       </c>
       <c r="C52" s="103"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="49"/>
+      <c r="D52" s="58">
+        <v>0</v>
+      </c>
+      <c r="E52" s="49">
+        <v>7.9118333333333331</v>
+      </c>
       <c r="F52" s="58">
         <f t="shared" ref="F52:F53" si="30">D52-E52</f>
-        <v>0</v>
+        <v>-7.9118333333333331</v>
       </c>
       <c r="G52" s="15">
         <v>384.9</v>
       </c>
-      <c r="H52" s="20"/>
+      <c r="H52" s="20">
+        <v>74</v>
+      </c>
       <c r="I52" s="16">
         <f>(D52*3600)/G52</f>
         <v>0</v>
       </c>
       <c r="J52" s="16">
         <f>I52-H52</f>
-        <v>0</v>
+        <v>-74</v>
       </c>
       <c r="K52" s="69" t="e">
         <f t="shared" ref="K52:K53" si="31">(N52+Q52)/D52</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L52" s="22"/>
+      <c r="L52" s="22">
+        <v>0</v>
+      </c>
       <c r="M52" s="53" t="e">
         <f>(N52/D52)*100%</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N52" s="48"/>
-      <c r="O52" s="23"/>
+      <c r="N52" s="48">
+        <v>0</v>
+      </c>
+      <c r="O52" s="23">
+        <v>0</v>
+      </c>
       <c r="P52" s="53" t="e">
         <f t="shared" ref="P52:P53" si="32">Q52/D52</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q52" s="48"/>
+      <c r="Q52" s="48">
+        <v>0</v>
+      </c>
       <c r="R52" s="50">
         <f t="shared" ref="R52:R53" si="33">F52-(Q52+N52)</f>
-        <v>0</v>
+        <v>-7.9118333333333331</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9825,43 +9875,57 @@
         <v>17</v>
       </c>
       <c r="C53" s="103"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="64"/>
+      <c r="D53" s="58">
+        <v>0</v>
+      </c>
+      <c r="E53" s="64">
+        <v>4.0628333333333329</v>
+      </c>
       <c r="F53" s="58">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>-4.0628333333333329</v>
       </c>
       <c r="G53" s="15">
         <v>384.9</v>
       </c>
-      <c r="H53" s="25"/>
+      <c r="H53" s="25">
+        <v>38</v>
+      </c>
       <c r="I53" s="16">
         <f>(D53*3600)/G53</f>
         <v>0</v>
       </c>
       <c r="J53" s="16">
         <f>I53-H53</f>
-        <v>0</v>
+        <v>-38</v>
       </c>
       <c r="K53" s="69" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L53" s="27"/>
+      <c r="L53" s="27">
+        <v>0</v>
+      </c>
       <c r="M53" s="53" t="e">
         <f>(N53/D53)*100%</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N53" s="62"/>
-      <c r="O53" s="28"/>
+      <c r="N53" s="62">
+        <v>0</v>
+      </c>
+      <c r="O53" s="28">
+        <v>0</v>
+      </c>
       <c r="P53" s="53" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q53" s="48"/>
+      <c r="Q53" s="48">
+        <v>0</v>
+      </c>
       <c r="R53" s="50">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>-4.0628333333333329</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9876,16 +9940,16 @@
       </c>
       <c r="E54" s="59">
         <f>SUM(E51:E53)</f>
-        <v>0</v>
+        <v>19.886499999999998</v>
       </c>
       <c r="F54" s="59">
         <f>SUM(F51:F53)</f>
-        <v>0</v>
+        <v>-19.886499999999998</v>
       </c>
       <c r="G54" s="31"/>
       <c r="H54" s="30">
         <f>SUM(H51:H53)</f>
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="I54" s="32">
         <f>SUM(I51:I53)</f>
@@ -9893,7 +9957,7 @@
       </c>
       <c r="J54" s="32">
         <f>SUM(J51:J53)</f>
-        <v>0</v>
+        <v>-186</v>
       </c>
       <c r="K54" s="33" t="e">
         <f>AVERAGE(K51:K53)</f>
@@ -9922,7 +9986,7 @@
       </c>
       <c r="R54" s="56">
         <f>SUM(R51:R53)</f>
-        <v>0</v>
+        <v>-19.886499999999998</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>